<commit_message>
added age group conditions
</commit_message>
<xml_diff>
--- a/Rating_BlockOrder.xlsx
+++ b/Rating_BlockOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelsielau/Ratings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C4DB8D-3E23-6A46-86C3-FF94674E0831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424CDEBE-B6AF-4F44-8CD9-A485D017B565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="15800" xr2:uid="{930A44AD-3E3D-CE45-9183-F4418BA56B34}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>RatingBlock</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>TrialCondition_B.xlsx</t>
+  </si>
+  <si>
+    <t>TrialCondition_C.xlsx</t>
+  </si>
+  <si>
+    <t>TrialCondition_D.xlsx</t>
+  </si>
+  <si>
+    <t>TrialCondition_E.xlsx</t>
+  </si>
+  <si>
+    <t>TrialCondition_F.xlsx</t>
   </si>
 </sst>
 </file>
@@ -401,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB48B7B-7EAA-E04C-B40E-BE008C743D38}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,6 +439,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>